<commit_message>
make full transfer into file report. and now its fully running now should to add error handling
</commit_message>
<xml_diff>
--- a/bot/Expenses.xlsx
+++ b/bot/Expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Дата</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>test33</t>
-  </si>
-  <si>
-    <t>test34</t>
   </si>
   <si>
     <t>Всього:</t>
@@ -435,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -782,32 +779,15 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
       <c r="C21" t="s">
         <v>28</v>
       </c>
       <c r="D21">
-        <v>3004</v>
+        <f>SUM(D2:D20)</f>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>72.66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="C22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22">
-        <f>SUM(D2:D21)</f>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f>SUM(E2:E21)</f>
+        <f>SUM(E2:E20)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add regexes to validate input to proper values now should make error response handlers
</commit_message>
<xml_diff>
--- a/bot/Expenses.xlsx
+++ b/bot/Expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Дата</t>
   </si>
@@ -31,73 +31,25 @@
     <t>Сума дол</t>
   </si>
   <si>
-    <t>2025-04-20</t>
-  </si>
-  <si>
-    <t>test00</t>
-  </si>
-  <si>
-    <t>test01</t>
-  </si>
-  <si>
-    <t>test02</t>
-  </si>
-  <si>
-    <t>test03</t>
-  </si>
-  <si>
-    <t>test04</t>
-  </si>
-  <si>
-    <t>2025-04-21</t>
-  </si>
-  <si>
-    <t>test20</t>
-  </si>
-  <si>
-    <t>test21</t>
-  </si>
-  <si>
-    <t>test22</t>
-  </si>
-  <si>
-    <t>test23</t>
-  </si>
-  <si>
-    <t>test24</t>
-  </si>
-  <si>
-    <t>2025-04-22</t>
-  </si>
-  <si>
-    <t>test10</t>
-  </si>
-  <si>
-    <t>test11</t>
-  </si>
-  <si>
-    <t>test12</t>
-  </si>
-  <si>
-    <t>test13</t>
-  </si>
-  <si>
-    <t>test14</t>
-  </si>
-  <si>
-    <t>2025-04-23</t>
-  </si>
-  <si>
-    <t>test30</t>
-  </si>
-  <si>
-    <t>test31</t>
-  </si>
-  <si>
-    <t>test32</t>
-  </si>
-  <si>
-    <t>test33</t>
+    <t>2020-11-11</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>2025-04-06</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>2025-12-13</t>
+  </si>
+  <si>
+    <t>test regex</t>
   </si>
   <si>
     <t>Всього:</t>
@@ -432,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,16 +412,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>1000.3</v>
+        <v>0.321</v>
       </c>
       <c r="E2">
-        <v>24.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -477,317 +429,62 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3">
-        <v>1001.3</v>
+        <v>-123</v>
       </c>
       <c r="E3">
-        <v>24.22</v>
+        <v>-2.98</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>1002.3</v>
+        <v>321</v>
       </c>
       <c r="E4">
-        <v>24.24</v>
+        <v>7.76</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>1003.3</v>
+        <v>700</v>
       </c>
       <c r="E5">
-        <v>24.27</v>
+        <v>16.93</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>1004.3</v>
+        <f>SUM(D2:D5)</f>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>24.29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>1000.4</v>
-      </c>
-      <c r="E7">
-        <v>24.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8">
-        <v>1001.4</v>
-      </c>
-      <c r="E8">
-        <v>24.22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9">
-        <v>1002.4</v>
-      </c>
-      <c r="E9">
-        <v>24.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>1003.4</v>
-      </c>
-      <c r="E10">
-        <v>24.27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>1004.4</v>
-      </c>
-      <c r="E11">
-        <v>24.29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12">
-        <v>1000</v>
-      </c>
-      <c r="E12">
-        <v>24.19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13">
-        <v>1001</v>
-      </c>
-      <c r="E13">
-        <v>24.21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14">
-        <v>1002</v>
-      </c>
-      <c r="E14">
-        <v>24.24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15">
-        <v>1003</v>
-      </c>
-      <c r="E15">
-        <v>24.26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16">
-        <v>1004</v>
-      </c>
-      <c r="E16">
-        <v>24.28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17">
-        <v>3000</v>
-      </c>
-      <c r="E17">
-        <v>72.56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18">
-        <v>3001</v>
-      </c>
-      <c r="E18">
-        <v>72.59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19">
-        <v>3002</v>
-      </c>
-      <c r="E19">
-        <v>72.61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20">
-        <v>3003</v>
-      </c>
-      <c r="E20">
-        <v>72.64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="C21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21">
-        <f>SUM(D2:D20)</f>
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <f>SUM(E2:E20)</f>
+        <f>SUM(E2:E5)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
i think for now its done
</commit_message>
<xml_diff>
--- a/bot/Expenses.xlsx
+++ b/bot/Expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Дата</t>
   </si>
@@ -31,25 +31,82 @@
     <t>Сума дол</t>
   </si>
   <si>
-    <t>2020-11-11</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>2025-04-06</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>2025-12-13</t>
-  </si>
-  <si>
-    <t>test regex</t>
+    <t>2025-04-20</t>
+  </si>
+  <si>
+    <t>test00</t>
+  </si>
+  <si>
+    <t>test01</t>
+  </si>
+  <si>
+    <t>test02</t>
+  </si>
+  <si>
+    <t>test03</t>
+  </si>
+  <si>
+    <t>test04</t>
+  </si>
+  <si>
+    <t>2025-04-21</t>
+  </si>
+  <si>
+    <t>test20</t>
+  </si>
+  <si>
+    <t>test21</t>
+  </si>
+  <si>
+    <t>test22</t>
+  </si>
+  <si>
+    <t>test23</t>
+  </si>
+  <si>
+    <t>test24</t>
+  </si>
+  <si>
+    <t>2025-04-22</t>
+  </si>
+  <si>
+    <t>test10</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>test13</t>
+  </si>
+  <si>
+    <t>test14</t>
+  </si>
+  <si>
+    <t>2025-04-23</t>
+  </si>
+  <si>
+    <t>test30</t>
+  </si>
+  <si>
+    <t>test31</t>
+  </si>
+  <si>
+    <t>test32</t>
+  </si>
+  <si>
+    <t>test33</t>
+  </si>
+  <si>
+    <t>2025-10-10</t>
+  </si>
+  <si>
+    <t>test exception</t>
+  </si>
+  <si>
+    <t>test exception 3</t>
   </si>
   <si>
     <t>Всього:</t>
@@ -384,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,10 +475,10 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>0.321</v>
+        <v>1000.3</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -435,56 +492,345 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>-123</v>
+        <v>1001.3</v>
       </c>
       <c r="E3">
-        <v>-2.98</v>
+        <v>24.22</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4">
-        <v>321</v>
+        <v>1002.3</v>
       </c>
       <c r="E4">
-        <v>7.76</v>
+        <v>24.24</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1003.3</v>
+      </c>
+      <c r="E5">
+        <v>24.27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D6">
+        <v>1004.3</v>
+      </c>
+      <c r="E6">
+        <v>24.29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
-        <v>700</v>
-      </c>
-      <c r="E5">
-        <v>16.93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="C6" t="s">
+      <c r="B7">
         <v>12</v>
       </c>
-      <c r="D6">
-        <f>SUM(D2:D5)</f>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1000.4</v>
+      </c>
+      <c r="E7">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>1001.4</v>
+      </c>
+      <c r="E8">
+        <v>24.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>1002.4</v>
+      </c>
+      <c r="E9">
+        <v>24.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>1003.4</v>
+      </c>
+      <c r="E10">
+        <v>24.27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>1004.4</v>
+      </c>
+      <c r="E11">
+        <v>24.29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>1000</v>
+      </c>
+      <c r="E12">
+        <v>24.19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>1001</v>
+      </c>
+      <c r="E13">
+        <v>24.21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>1002</v>
+      </c>
+      <c r="E14">
+        <v>24.24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15">
+        <v>1003</v>
+      </c>
+      <c r="E15">
+        <v>24.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>1004</v>
+      </c>
+      <c r="E16">
+        <v>24.28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>3000</v>
+      </c>
+      <c r="E17">
+        <v>72.56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>3001</v>
+      </c>
+      <c r="E18">
+        <v>72.59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19">
+        <v>3002</v>
+      </c>
+      <c r="E19">
+        <v>72.61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20">
+        <v>3003</v>
+      </c>
+      <c r="E20">
+        <v>72.64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <v>400</v>
+      </c>
+      <c r="E21">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>400</v>
+      </c>
+      <c r="E22">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <f>SUM(D2:D22)</f>
         <v>0</v>
       </c>
-      <c r="E6">
-        <f>SUM(E2:E5)</f>
+      <c r="E23">
+        <f>SUM(E2:E22)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>